<commit_message>
basically working. fade control still need work.
</commit_message>
<xml_diff>
--- a/IR remote codes.xlsx
+++ b/IR remote codes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/Documents/Arduino/led_strip_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED8C171-B025-E14E-8850-F2AC3F8810E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F320C4A-C3AA-C246-909E-D05E5BEE0F5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7960" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{B5F908D1-F10E-1240-83B3-DB22BBEC8620}"/>
+    <workbookView xWindow="11540" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{B5F908D1-F10E-1240-83B3-DB22BBEC8620}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="black elgo" sheetId="1" r:id="rId1"/>
+    <sheet name="Snapper" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Power</t>
   </si>
@@ -131,9 +132,6 @@
     <t>FF52AD</t>
   </si>
   <si>
-    <t>(copied from monitor)</t>
-  </si>
-  <si>
     <t>MAP</t>
   </si>
   <si>
@@ -159,6 +157,54 @@
   </si>
   <si>
     <t>all on</t>
+  </si>
+  <si>
+    <t>bright up</t>
+  </si>
+  <si>
+    <t>bright down</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>flash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row </t>
+  </si>
+  <si>
+    <t>strobe</t>
+  </si>
+  <si>
+    <t>fade</t>
+  </si>
+  <si>
+    <t>smooth</t>
+  </si>
+  <si>
+    <t>Colors designate columns via the first row buttons</t>
+  </si>
+  <si>
+    <t>NB, several red column buttons do not work</t>
+  </si>
+  <si>
+    <t>int values</t>
   </si>
 </sst>
 </file>
@@ -513,17 +559,17 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -534,7 +580,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>16753245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -544,8 +593,8 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
+      <c r="D3">
+        <v>16736925</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -556,10 +605,10 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>39</v>
+      </c>
+      <c r="D4">
+        <v>16769565</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -569,8 +618,8 @@
       <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
+      <c r="D5">
+        <v>16720605</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -580,8 +629,8 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
+      <c r="D6">
+        <v>16712445</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -591,8 +640,8 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
+      <c r="D7">
+        <v>16761405</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -602,8 +651,8 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
+      <c r="D8">
+        <v>16769055</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -613,8 +662,8 @@
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
+      <c r="D9">
+        <v>16754775</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -624,8 +673,8 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" t="s">
-        <v>19</v>
+      <c r="D10">
+        <v>16748655</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -635,8 +684,8 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
-        <v>20</v>
+      <c r="D11">
+        <v>16738455</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -646,8 +695,8 @@
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>21</v>
+      <c r="D12">
+        <v>16750695</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -657,8 +706,8 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
-        <v>22</v>
+      <c r="D13">
+        <v>16756815</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -669,10 +718,10 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>16724175</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -683,10 +732,10 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>16718055</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -697,10 +746,10 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="D16">
+        <v>16743045</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -711,10 +760,10 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>16716015</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -725,10 +774,10 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>16726215</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -739,10 +788,10 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>16734885</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -752,8 +801,8 @@
       <c r="B20" t="s">
         <v>29</v>
       </c>
-      <c r="D20" t="s">
-        <v>29</v>
+      <c r="D20">
+        <v>16728765</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -763,8 +812,8 @@
       <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="D21" t="s">
-        <v>30</v>
+      <c r="D21">
+        <v>16730805</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -774,12 +823,290 @@
       <c r="B22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" t="s">
-        <v>31</v>
+      <c r="D22">
+        <v>16732845</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9302AAE-AC2B-3A4A-B082-C382196F3581}">
+  <dimension ref="B1:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>16187647</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>16220287</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>16203967</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>16236599</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>16220287</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>16187647</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>16244759</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>16212127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>16228447</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>16195807</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>16240675</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>16208047</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>16224359</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>16248839</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>16248972</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>16232527</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>16199887</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>16238647</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>16206007</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>16222327</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>16246790</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>16246933</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>16230470</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>16246918</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>